<commit_message>
Finish Webb, Christie, and Bush
</commit_message>
<xml_diff>
--- a/data/GoodCSVs/ChrisChristie.xlsx
+++ b/data/GoodCSVs/ChrisChristie.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\campaign-contributions\data\GoodCSVs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="21075" windowHeight="9780"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -766,6 +771,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -813,7 +821,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -848,7 +856,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1060,7 +1068,8 @@
   <dimension ref="A1:Q53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,26 +1162,25 @@
         <v>0</v>
       </c>
       <c r="K2" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L2" s="5">
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="M2" s="5">
-        <v>0</v>
+        <v>875</v>
       </c>
       <c r="N2" s="5">
-        <v>0</v>
+        <v>1275</v>
       </c>
       <c r="O2" s="5">
-        <v>0</v>
+        <v>1125</v>
       </c>
       <c r="P2" s="5">
         <v>0</v>
       </c>
       <c r="Q2" s="5">
-        <f>SUM(F2:P2)</f>
-        <v>0</v>
+        <v>3645</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -1207,13 +1215,13 @@
         <v>0</v>
       </c>
       <c r="K3" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L3" s="5">
         <v>0</v>
       </c>
       <c r="M3" s="5">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N3" s="5">
         <v>0</v>
@@ -1225,8 +1233,7 @@
         <v>0</v>
       </c>
       <c r="Q3" s="5">
-        <f t="shared" ref="Q3:Q52" si="0">SUM(F3:P3)</f>
-        <v>0</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1261,26 +1268,25 @@
         <v>1100</v>
       </c>
       <c r="K4" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="L4" s="5">
-        <v>0</v>
+        <v>42200</v>
       </c>
       <c r="M4" s="5">
-        <v>0</v>
+        <v>8050</v>
       </c>
       <c r="N4" s="5">
-        <v>0</v>
+        <v>1650</v>
       </c>
       <c r="O4" s="5">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="P4" s="5">
         <v>0</v>
       </c>
       <c r="Q4" s="5">
-        <f t="shared" si="0"/>
-        <v>5550</v>
+        <v>57850</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1315,16 +1321,16 @@
         <v>3200</v>
       </c>
       <c r="K5" s="5">
-        <v>0</v>
+        <v>2700</v>
       </c>
       <c r="L5" s="5">
-        <v>0</v>
+        <v>5400</v>
       </c>
       <c r="M5" s="5">
-        <v>0</v>
+        <v>5400</v>
       </c>
       <c r="N5" s="5">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="O5" s="5">
         <v>0</v>
@@ -1333,8 +1339,7 @@
         <v>0</v>
       </c>
       <c r="Q5" s="5">
-        <f t="shared" si="0"/>
-        <v>8600</v>
+        <v>22600</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -1366,29 +1371,28 @@
         <v>16400</v>
       </c>
       <c r="J6" s="5">
-        <v>0</v>
+        <v>42900</v>
       </c>
       <c r="K6" s="5">
-        <v>0</v>
+        <v>55600</v>
       </c>
       <c r="L6" s="5">
-        <v>0</v>
+        <v>73625</v>
       </c>
       <c r="M6" s="5">
-        <v>0</v>
+        <v>167025</v>
       </c>
       <c r="N6" s="5">
-        <v>0</v>
+        <v>29391</v>
       </c>
       <c r="O6" s="5">
-        <v>0</v>
+        <v>6575</v>
       </c>
       <c r="P6" s="5">
         <v>0</v>
       </c>
       <c r="Q6" s="5">
-        <f t="shared" si="0"/>
-        <v>59550</v>
+        <v>434666</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1420,29 +1424,28 @@
         <v>0</v>
       </c>
       <c r="J7" s="5">
-        <v>0</v>
+        <v>3200</v>
       </c>
       <c r="K7" s="5">
-        <v>0</v>
+        <v>18109</v>
       </c>
       <c r="L7" s="5">
-        <v>0</v>
+        <v>10125</v>
       </c>
       <c r="M7" s="5">
-        <v>0</v>
+        <v>1175</v>
       </c>
       <c r="N7" s="5">
-        <v>0</v>
+        <v>8900</v>
       </c>
       <c r="O7" s="5">
-        <v>0</v>
+        <v>14400</v>
       </c>
       <c r="P7" s="5">
         <v>0</v>
       </c>
       <c r="Q7" s="5">
-        <f t="shared" si="0"/>
-        <v>8630</v>
+        <v>64539</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1474,29 +1477,28 @@
         <v>10940.38</v>
       </c>
       <c r="J8" s="5">
-        <v>0</v>
+        <v>65529.62</v>
       </c>
       <c r="K8" s="5">
-        <v>0</v>
+        <v>28300</v>
       </c>
       <c r="L8" s="5">
-        <v>0</v>
+        <v>58100</v>
       </c>
       <c r="M8" s="5">
-        <v>0</v>
+        <v>20425</v>
       </c>
       <c r="N8" s="5">
-        <v>0</v>
+        <v>11425</v>
       </c>
       <c r="O8" s="5">
-        <v>0</v>
+        <v>13275</v>
       </c>
       <c r="P8" s="5">
         <v>0</v>
       </c>
       <c r="Q8" s="5">
-        <f t="shared" si="0"/>
-        <v>36270.379999999997</v>
+        <v>233325</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -1528,29 +1530,28 @@
         <v>0</v>
       </c>
       <c r="J9" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="K9" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L9" s="5">
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="M9" s="5">
         <v>0</v>
       </c>
       <c r="N9" s="5">
-        <v>0</v>
+        <v>675</v>
       </c>
       <c r="O9" s="5">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P9" s="5">
         <v>0</v>
       </c>
       <c r="Q9" s="5">
-        <f t="shared" si="0"/>
-        <v>3200</v>
+        <v>5775</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -1582,29 +1583,28 @@
         <v>8600</v>
       </c>
       <c r="J10" s="5">
-        <v>0</v>
+        <v>9600</v>
       </c>
       <c r="K10" s="5">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="L10" s="5">
-        <v>0</v>
+        <v>3550</v>
       </c>
       <c r="M10" s="5">
-        <v>0</v>
+        <v>11350</v>
       </c>
       <c r="N10" s="5">
-        <v>0</v>
+        <v>4350</v>
       </c>
       <c r="O10" s="5">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P10" s="5">
         <v>0</v>
       </c>
       <c r="Q10" s="5">
-        <f t="shared" si="0"/>
-        <v>15500</v>
+        <v>45150</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1636,29 +1636,28 @@
         <v>27900</v>
       </c>
       <c r="J11" s="5">
-        <v>0</v>
+        <v>29500</v>
       </c>
       <c r="K11" s="5">
-        <v>0</v>
+        <v>12453</v>
       </c>
       <c r="L11" s="5">
-        <v>0</v>
+        <v>25700</v>
       </c>
       <c r="M11" s="5">
-        <v>0</v>
+        <v>87350</v>
       </c>
       <c r="N11" s="5">
-        <v>0</v>
+        <v>13626.25</v>
       </c>
       <c r="O11" s="5">
-        <v>0</v>
+        <v>7300</v>
       </c>
       <c r="P11" s="5">
         <v>0</v>
       </c>
       <c r="Q11" s="5">
-        <f t="shared" si="0"/>
-        <v>93900</v>
+        <v>269829.25</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1690,29 +1689,28 @@
         <v>2600</v>
       </c>
       <c r="J12" s="5">
-        <v>0</v>
+        <v>10303</v>
       </c>
       <c r="K12" s="5">
-        <v>0</v>
+        <v>2750</v>
       </c>
       <c r="L12" s="5">
-        <v>0</v>
+        <v>3325</v>
       </c>
       <c r="M12" s="5">
-        <v>0</v>
+        <v>6325</v>
       </c>
       <c r="N12" s="5">
-        <v>0</v>
+        <v>2775</v>
       </c>
       <c r="O12" s="5">
-        <v>0</v>
+        <v>4950</v>
       </c>
       <c r="P12" s="5">
         <v>0</v>
       </c>
       <c r="Q12" s="5">
-        <f t="shared" si="0"/>
-        <v>4700</v>
+        <v>35128</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1765,7 +1763,6 @@
         <v>0</v>
       </c>
       <c r="Q13" s="5">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1810,17 +1807,16 @@
         <v>0</v>
       </c>
       <c r="N14" s="5">
-        <v>0</v>
+        <v>2871</v>
       </c>
       <c r="O14" s="5">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="P14" s="5">
         <v>0</v>
       </c>
       <c r="Q14" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3071</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1852,29 +1848,28 @@
         <v>16450</v>
       </c>
       <c r="J15" s="5">
-        <v>0</v>
+        <v>44000</v>
       </c>
       <c r="K15" s="5">
-        <v>0</v>
+        <v>22913</v>
       </c>
       <c r="L15" s="5">
-        <v>0</v>
+        <v>1110</v>
       </c>
       <c r="M15" s="5">
-        <v>0</v>
+        <v>4725</v>
       </c>
       <c r="N15" s="5">
-        <v>0</v>
+        <v>34725</v>
       </c>
       <c r="O15" s="5">
-        <v>0</v>
+        <v>8650</v>
       </c>
       <c r="P15" s="5">
         <v>0</v>
       </c>
       <c r="Q15" s="5">
-        <f t="shared" si="0"/>
-        <v>30250</v>
+        <v>146373</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -1906,19 +1901,19 @@
         <v>0</v>
       </c>
       <c r="J16" s="5">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="K16" s="5">
-        <v>0</v>
+        <v>17200</v>
       </c>
       <c r="L16" s="5">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="M16" s="5">
-        <v>0</v>
+        <v>1525</v>
       </c>
       <c r="N16" s="5">
-        <v>0</v>
+        <v>4300</v>
       </c>
       <c r="O16" s="5">
         <v>0</v>
@@ -1927,8 +1922,7 @@
         <v>0</v>
       </c>
       <c r="Q16" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>24525</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -1960,29 +1954,28 @@
         <v>0</v>
       </c>
       <c r="J17" s="5">
-        <v>0</v>
+        <v>7425</v>
       </c>
       <c r="K17" s="5">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="L17" s="5">
-        <v>0</v>
+        <v>2700</v>
       </c>
       <c r="M17" s="5">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="N17" s="5">
-        <v>0</v>
+        <v>38850</v>
       </c>
       <c r="O17" s="5">
-        <v>0</v>
+        <v>5650</v>
       </c>
       <c r="P17" s="5">
         <v>0</v>
       </c>
       <c r="Q17" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>58625</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -2017,26 +2010,25 @@
         <v>0</v>
       </c>
       <c r="K18" s="5">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L18" s="5">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="M18" s="5">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="N18" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O18" s="5">
-        <v>0</v>
+        <v>2750</v>
       </c>
       <c r="P18" s="5">
         <v>0</v>
       </c>
       <c r="Q18" s="5">
-        <f t="shared" si="0"/>
-        <v>5400</v>
+        <v>8475</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -2077,20 +2069,19 @@
         <v>0</v>
       </c>
       <c r="M19" s="5">
-        <v>0</v>
+        <v>5200</v>
       </c>
       <c r="N19" s="5">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="O19" s="5">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="P19" s="5">
         <v>0</v>
       </c>
       <c r="Q19" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5550</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -2134,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="N20" s="5">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="O20" s="5">
         <v>0</v>
@@ -2143,8 +2134,7 @@
         <v>0</v>
       </c>
       <c r="Q20" s="5">
-        <f t="shared" si="0"/>
-        <v>2700</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -2176,29 +2166,28 @@
         <v>0</v>
       </c>
       <c r="J21" s="5">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="K21" s="5">
-        <v>0</v>
+        <v>5400</v>
       </c>
       <c r="L21" s="5">
-        <v>0</v>
+        <v>1600</v>
       </c>
       <c r="M21" s="5">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="N21" s="5">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="O21" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="P21" s="5">
         <v>0</v>
       </c>
       <c r="Q21" s="5">
-        <f t="shared" si="0"/>
-        <v>250</v>
+        <v>8700</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -2230,29 +2219,28 @@
         <v>82550</v>
       </c>
       <c r="J22" s="5">
-        <v>0</v>
+        <v>31503</v>
       </c>
       <c r="K22" s="5">
-        <v>0</v>
+        <v>7255</v>
       </c>
       <c r="L22" s="5">
-        <v>0</v>
+        <v>4425</v>
       </c>
       <c r="M22" s="5">
-        <v>0</v>
+        <v>28100</v>
       </c>
       <c r="N22" s="5">
-        <v>0</v>
+        <v>60600</v>
       </c>
       <c r="O22" s="5">
-        <v>0</v>
+        <v>10400</v>
       </c>
       <c r="P22" s="5">
         <v>0</v>
       </c>
       <c r="Q22" s="5">
-        <f t="shared" si="0"/>
-        <v>92400</v>
+        <v>234683</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -2284,29 +2272,28 @@
         <v>28700</v>
       </c>
       <c r="J23" s="5">
-        <v>0</v>
+        <v>46570</v>
       </c>
       <c r="K23" s="5">
-        <v>0</v>
+        <v>21350</v>
       </c>
       <c r="L23" s="5">
-        <v>0</v>
+        <v>7850</v>
       </c>
       <c r="M23" s="5">
-        <v>0</v>
+        <v>17300</v>
       </c>
       <c r="N23" s="5">
-        <v>0</v>
+        <v>1875</v>
       </c>
       <c r="O23" s="5">
-        <v>0</v>
+        <v>15425</v>
       </c>
       <c r="P23" s="5">
         <v>0</v>
       </c>
       <c r="Q23" s="5">
-        <f t="shared" si="0"/>
-        <v>45750</v>
+        <v>156120</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -2338,29 +2325,28 @@
         <v>2700</v>
       </c>
       <c r="J24" s="5">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="K24" s="5">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L24" s="5">
-        <v>0</v>
+        <v>3200</v>
       </c>
       <c r="M24" s="5">
-        <v>0</v>
+        <v>5325</v>
       </c>
       <c r="N24" s="5">
-        <v>0</v>
+        <v>5400</v>
       </c>
       <c r="O24" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="P24" s="5">
         <v>0</v>
       </c>
       <c r="Q24" s="5">
-        <f t="shared" si="0"/>
-        <v>6900</v>
+        <v>21625</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -2392,29 +2378,28 @@
         <v>3950</v>
       </c>
       <c r="J25" s="5">
-        <v>0</v>
+        <v>25800</v>
       </c>
       <c r="K25" s="5">
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="L25" s="5">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="M25" s="5">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="N25" s="5">
-        <v>0</v>
+        <v>1250</v>
       </c>
       <c r="O25" s="5">
-        <v>0</v>
+        <v>3900</v>
       </c>
       <c r="P25" s="5">
         <v>0</v>
       </c>
       <c r="Q25" s="5">
-        <f t="shared" si="0"/>
-        <v>9175</v>
+        <v>41128</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -2467,7 +2452,6 @@
         <v>0</v>
       </c>
       <c r="Q26" s="5">
-        <f t="shared" si="0"/>
         <v>3700</v>
       </c>
     </row>
@@ -2500,29 +2484,28 @@
         <v>0</v>
       </c>
       <c r="J27" s="5">
-        <v>0</v>
+        <v>21700</v>
       </c>
       <c r="K27" s="5">
-        <v>0</v>
+        <v>35700</v>
       </c>
       <c r="L27" s="5">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="M27" s="5">
-        <v>0</v>
+        <v>1701</v>
       </c>
       <c r="N27" s="5">
-        <v>0</v>
+        <v>-2555</v>
       </c>
       <c r="O27" s="5">
-        <v>0</v>
+        <v>3815</v>
       </c>
       <c r="P27" s="5">
         <v>0</v>
       </c>
       <c r="Q27" s="5">
-        <f t="shared" si="0"/>
-        <v>5400</v>
+        <v>70761</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -2560,13 +2543,13 @@
         <v>0</v>
       </c>
       <c r="L28" s="5">
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="M28" s="5">
-        <v>0</v>
+        <v>1700</v>
       </c>
       <c r="N28" s="5">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O28" s="5">
         <v>0</v>
@@ -2575,8 +2558,7 @@
         <v>0</v>
       </c>
       <c r="Q28" s="5">
-        <f t="shared" si="0"/>
-        <v>750</v>
+        <v>3400</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -2620,7 +2602,7 @@
         <v>0</v>
       </c>
       <c r="N29" s="5">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="O29" s="5">
         <v>0</v>
@@ -2629,8 +2611,7 @@
         <v>0</v>
       </c>
       <c r="Q29" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -2662,29 +2643,28 @@
         <v>350</v>
       </c>
       <c r="J30" s="5">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="K30" s="5">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="L30" s="5">
-        <v>0</v>
+        <v>5900</v>
       </c>
       <c r="M30" s="5">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="N30" s="5">
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="O30" s="5">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="P30" s="5">
         <v>0</v>
       </c>
       <c r="Q30" s="5">
-        <f t="shared" si="0"/>
-        <v>3150</v>
+        <v>15150</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -2716,29 +2696,28 @@
         <v>1500</v>
       </c>
       <c r="J31" s="5">
-        <v>0</v>
+        <v>6500</v>
       </c>
       <c r="K31" s="5">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="L31" s="5">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="M31" s="5">
-        <v>0</v>
+        <v>9400</v>
       </c>
       <c r="N31" s="5">
-        <v>0</v>
+        <v>9325</v>
       </c>
       <c r="O31" s="5">
-        <v>0</v>
+        <v>8095.16</v>
       </c>
       <c r="P31" s="5">
         <v>0</v>
       </c>
       <c r="Q31" s="5">
-        <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>35920.160000000003</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -2770,29 +2749,28 @@
         <v>537700</v>
       </c>
       <c r="J32" s="5">
-        <v>0</v>
+        <v>635556.13</v>
       </c>
       <c r="K32" s="5">
-        <v>0</v>
+        <v>248086</v>
       </c>
       <c r="L32" s="5">
-        <v>0</v>
+        <v>216070</v>
       </c>
       <c r="M32" s="5">
-        <v>0</v>
+        <v>613385</v>
       </c>
       <c r="N32" s="5">
-        <v>0</v>
+        <v>215953.22</v>
       </c>
       <c r="O32" s="5">
-        <v>0</v>
+        <v>106778.88</v>
       </c>
       <c r="P32" s="5">
         <v>0</v>
       </c>
       <c r="Q32" s="5">
-        <f t="shared" si="0"/>
-        <v>1560105</v>
+        <v>3595934.23</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -2845,7 +2823,6 @@
         <v>0</v>
       </c>
       <c r="Q33" s="5">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2878,29 +2855,28 @@
         <v>115520</v>
       </c>
       <c r="J34" s="5">
-        <v>0</v>
+        <v>163311</v>
       </c>
       <c r="K34" s="5">
-        <v>0</v>
+        <v>38375</v>
       </c>
       <c r="L34" s="5">
-        <v>0</v>
+        <v>85575</v>
       </c>
       <c r="M34" s="5">
-        <v>0</v>
+        <v>191475</v>
       </c>
       <c r="N34" s="5">
-        <v>0</v>
+        <v>77356</v>
       </c>
       <c r="O34" s="5">
-        <v>0</v>
+        <v>52725</v>
       </c>
       <c r="P34" s="5">
         <v>0</v>
       </c>
       <c r="Q34" s="5">
-        <f t="shared" si="0"/>
-        <v>226970</v>
+        <v>835787</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -2932,29 +2908,28 @@
         <v>0</v>
       </c>
       <c r="J35" s="5">
-        <v>0</v>
+        <v>5900</v>
       </c>
       <c r="K35" s="5">
-        <v>0</v>
+        <v>3150</v>
       </c>
       <c r="L35" s="5">
-        <v>0</v>
+        <v>2195</v>
       </c>
       <c r="M35" s="5">
-        <v>0</v>
+        <v>1050</v>
       </c>
       <c r="N35" s="5">
-        <v>0</v>
+        <v>6500</v>
       </c>
       <c r="O35" s="5">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="P35" s="5">
         <v>0</v>
       </c>
       <c r="Q35" s="5">
-        <f t="shared" si="0"/>
-        <v>500</v>
+        <v>19495</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -3007,7 +2982,6 @@
         <v>0</v>
       </c>
       <c r="Q36" s="5">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3040,29 +3014,28 @@
         <v>0</v>
       </c>
       <c r="J37" s="5">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="K37" s="5">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="L37" s="5">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="M37" s="5">
-        <v>0</v>
+        <v>4600</v>
       </c>
       <c r="N37" s="5">
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="O37" s="5">
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="P37" s="5">
         <v>0</v>
       </c>
       <c r="Q37" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6200</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -3097,16 +3070,16 @@
         <v>0</v>
       </c>
       <c r="K38" s="5">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="L38" s="5">
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="M38" s="5">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="N38" s="5">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="O38" s="5">
         <v>0</v>
@@ -3115,8 +3088,7 @@
         <v>0</v>
       </c>
       <c r="Q38" s="5">
-        <f t="shared" si="0"/>
-        <v>500</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -3154,23 +3126,22 @@
         <v>0</v>
       </c>
       <c r="L39" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M39" s="5">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="N39" s="5">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="O39" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="P39" s="5">
         <v>0</v>
       </c>
       <c r="Q39" s="5">
-        <f t="shared" si="0"/>
-        <v>7400</v>
+        <v>8450</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -3202,29 +3173,28 @@
         <v>38750</v>
       </c>
       <c r="J40" s="5">
-        <v>0</v>
+        <v>26500</v>
       </c>
       <c r="K40" s="5">
-        <v>0</v>
+        <v>4475</v>
       </c>
       <c r="L40" s="5">
-        <v>0</v>
+        <v>67500</v>
       </c>
       <c r="M40" s="5">
-        <v>0</v>
+        <v>80050</v>
       </c>
       <c r="N40" s="5">
-        <v>0</v>
+        <v>93801</v>
       </c>
       <c r="O40" s="5">
-        <v>0</v>
+        <v>27990</v>
       </c>
       <c r="P40" s="5">
         <v>0</v>
       </c>
       <c r="Q40" s="5">
-        <f t="shared" si="0"/>
-        <v>87125</v>
+        <v>387441</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -3256,19 +3226,19 @@
         <v>0</v>
       </c>
       <c r="J41" s="5">
-        <v>0</v>
+        <v>5400</v>
       </c>
       <c r="K41" s="5">
         <v>0</v>
       </c>
       <c r="L41" s="5">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="M41" s="5">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="N41" s="5">
-        <v>0</v>
+        <v>775</v>
       </c>
       <c r="O41" s="5">
         <v>0</v>
@@ -3277,8 +3247,7 @@
         <v>0</v>
       </c>
       <c r="Q41" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7675</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -3310,29 +3279,28 @@
         <v>0</v>
       </c>
       <c r="J42" s="5">
-        <v>0</v>
+        <v>1750</v>
       </c>
       <c r="K42" s="5">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="L42" s="5">
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="M42" s="5">
-        <v>0</v>
+        <v>4100</v>
       </c>
       <c r="N42" s="5">
-        <v>0</v>
+        <v>1150</v>
       </c>
       <c r="O42" s="5">
-        <v>0</v>
+        <v>450</v>
       </c>
       <c r="P42" s="5">
         <v>0</v>
       </c>
       <c r="Q42" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9050</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -3373,7 +3341,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="5">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="N43" s="5">
         <v>0</v>
@@ -3385,8 +3353,7 @@
         <v>0</v>
       </c>
       <c r="Q43" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
@@ -3418,29 +3385,28 @@
         <v>10600</v>
       </c>
       <c r="J44" s="5">
-        <v>0</v>
+        <v>9650</v>
       </c>
       <c r="K44" s="5">
         <v>0</v>
       </c>
       <c r="L44" s="5">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="M44" s="5">
-        <v>0</v>
+        <v>3200</v>
       </c>
       <c r="N44" s="5">
-        <v>0</v>
+        <v>4325</v>
       </c>
       <c r="O44" s="5">
-        <v>0</v>
+        <v>2800</v>
       </c>
       <c r="P44" s="5">
         <v>0</v>
       </c>
       <c r="Q44" s="5">
-        <f t="shared" si="0"/>
-        <v>21400</v>
+        <v>41875</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
@@ -3472,29 +3438,28 @@
         <v>17845</v>
       </c>
       <c r="J45" s="5">
-        <v>0</v>
+        <v>128450</v>
       </c>
       <c r="K45" s="5">
-        <v>0</v>
+        <v>7725</v>
       </c>
       <c r="L45" s="5">
-        <v>0</v>
+        <v>7350</v>
       </c>
       <c r="M45" s="5">
-        <v>0</v>
+        <v>6975</v>
       </c>
       <c r="N45" s="5">
-        <v>0</v>
+        <v>30685</v>
       </c>
       <c r="O45" s="5">
-        <v>0</v>
+        <v>8275</v>
       </c>
       <c r="P45" s="5">
         <v>0</v>
       </c>
       <c r="Q45" s="5">
-        <f t="shared" si="0"/>
-        <v>73745</v>
+        <v>263205</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
@@ -3529,26 +3494,25 @@
         <v>0</v>
       </c>
       <c r="K46" s="5">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="L46" s="5">
         <v>0</v>
       </c>
       <c r="M46" s="5">
-        <v>0</v>
+        <v>-1400</v>
       </c>
       <c r="N46" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O46" s="5">
-        <v>0</v>
+        <v>2700</v>
       </c>
       <c r="P46" s="5">
         <v>0</v>
       </c>
       <c r="Q46" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
@@ -3583,7 +3547,7 @@
         <v>0</v>
       </c>
       <c r="K47" s="5">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="L47" s="5">
         <v>0</v>
@@ -3601,8 +3565,7 @@
         <v>0</v>
       </c>
       <c r="Q47" s="5">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
@@ -3634,29 +3597,28 @@
         <v>17520</v>
       </c>
       <c r="J48" s="5">
-        <v>0</v>
+        <v>46090</v>
       </c>
       <c r="K48" s="5">
-        <v>0</v>
+        <v>18250</v>
       </c>
       <c r="L48" s="5">
-        <v>0</v>
+        <v>4849</v>
       </c>
       <c r="M48" s="5">
-        <v>0</v>
+        <v>35965</v>
       </c>
       <c r="N48" s="5">
-        <v>0</v>
+        <v>10301</v>
       </c>
       <c r="O48" s="5">
-        <v>0</v>
+        <v>22475</v>
       </c>
       <c r="P48" s="5">
         <v>0</v>
       </c>
       <c r="Q48" s="5">
-        <f t="shared" si="0"/>
-        <v>49370</v>
+        <v>187300</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
@@ -3688,29 +3650,28 @@
         <v>0</v>
       </c>
       <c r="J49" s="5">
-        <v>0</v>
+        <v>2700</v>
       </c>
       <c r="K49" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="L49" s="5">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="M49" s="5">
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="N49" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="O49" s="5">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P49" s="5">
         <v>0</v>
       </c>
       <c r="Q49" s="5">
-        <f t="shared" si="0"/>
-        <v>500</v>
+        <v>4325</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
@@ -3748,13 +3709,13 @@
         <v>0</v>
       </c>
       <c r="L50" s="5">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="M50" s="5">
         <v>0</v>
       </c>
       <c r="N50" s="5">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="O50" s="5">
         <v>0</v>
@@ -3763,8 +3724,7 @@
         <v>0</v>
       </c>
       <c r="Q50" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
@@ -3796,29 +3756,28 @@
         <v>0</v>
       </c>
       <c r="J51" s="5">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="K51" s="5">
         <v>0</v>
       </c>
       <c r="L51" s="5">
-        <v>0</v>
+        <v>1250</v>
       </c>
       <c r="M51" s="5">
         <v>0</v>
       </c>
       <c r="N51" s="5">
-        <v>0</v>
+        <v>5400</v>
       </c>
       <c r="O51" s="5">
-        <v>0</v>
+        <v>3050</v>
       </c>
       <c r="P51" s="5">
         <v>0</v>
       </c>
       <c r="Q51" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10700</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
@@ -3853,7 +3812,7 @@
         <v>0</v>
       </c>
       <c r="K52" s="5">
-        <v>0</v>
+        <v>2700</v>
       </c>
       <c r="L52" s="5">
         <v>0</v>
@@ -3862,7 +3821,7 @@
         <v>0</v>
       </c>
       <c r="N52" s="5">
-        <v>0</v>
+        <v>2700</v>
       </c>
       <c r="O52" s="5">
         <v>0</v>
@@ -3871,59 +3830,21 @@
         <v>0</v>
       </c>
       <c r="Q52" s="5">
-        <f t="shared" si="0"/>
-        <v>2901</v>
+        <v>8301</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F53">
-        <f>SUM(F2:F52)</f>
-        <v>0</v>
-      </c>
-      <c r="G53" s="1">
-        <f t="shared" ref="G53:Q53" si="1">SUM(G2:G52)</f>
-        <v>0</v>
-      </c>
-      <c r="H53" s="1">
-        <f t="shared" si="1"/>
-        <v>1521966</v>
-      </c>
-      <c r="I53" s="1">
-        <f>SUM(I2:I52)+8100</f>
-        <v>956575.38</v>
-      </c>
-      <c r="J53" s="1">
-        <f t="shared" si="1"/>
-        <v>4300</v>
-      </c>
-      <c r="K53" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L53" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M53" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N53" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O53" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P53" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q53" s="1">
-        <f t="shared" si="1"/>
-        <v>2474741.38</v>
-      </c>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>